<commit_message>
feat: include YUV-PSNR in HEVC output:
</commit_message>
<xml_diff>
--- a/playground/HEVC_output.xlsx
+++ b/playground/HEVC_output.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\workspace\dip\playground\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{444E0B47-BA14-43BD-B706-9AEBD9CF6554}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{0415870B-3B88-4694-B3CA-AD7C12653B24}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="9585" xr2:uid="{23CED400-0C25-4AD2-A375-A3192218FF0C}"/>
   </bookViews>
@@ -371,15 +371,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD80C710-D246-4C26-BD88-8C132316A1A1}">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C1"/>
+      <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>456.36599999999999</v>
       </c>
@@ -389,6 +389,9 @@
       <c r="C1">
         <v>34.271999999999998</v>
       </c>
+      <c r="D1">
+        <v>33.748199999999997</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>